<commit_message>
and 0.0.x to version names
</commit_message>
<xml_diff>
--- a/system_development/V0.3.1/bill_of_materials.xlsx
+++ b/system_development/V0.3.1/bill_of_materials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailsc-my.sharepoint.com/personal/asifuzzaman_sc_edu/Documents/Github Repos/Sensor-Package-Access-Hub/system_development/V0.3.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Sensor-Package-Access-Hub\system_development\V0.3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{92FC9251-22EE-4CB6-81B0-D0434CABC585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E484CD04-FA4F-4275-ABDC-02BD98B955A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5E4ADA-0549-4EDF-861D-B013FD1FB40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="bill_of_materials" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -146,9 +146,6 @@
     <t>https://www.mouser.com/ProductDetail/Raspberry-Pi/SC01949?qs=T%252BzbugeAwjjISb%252BwlagpRw%3D%3D</t>
   </si>
   <si>
-    <t>NRF24</t>
-  </si>
-  <si>
     <t>https://www.elecbee.com/en/product-detail/1100-meter-long-distance-nrf24l01-pa-lna-wireless-module-with-antenna-module_73275?utm_term=&amp;utm_campaign=&amp;utm_source=adwords&amp;utm_medium=ppc&amp;hsa_acc=9958698819&amp;hsa_cam=23146566611&amp;hsa_grp=187297116859&amp;hsa_ad=779498650524&amp;hsa_src=g&amp;hsa_tgt=pla-2511885727437&amp;hsa_kw=&amp;hsa_mt=&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gad_source=1&amp;gad_campaignid=23146566611&amp;gbraid=0AAAAADGHwHYfKF0iMEZtoqyx1rWjzHw1t&amp;gclid=Cj0KCQiA5abIBhCaARIsAM3-zFXbXR-v0fRxqHBuXN-ZMrGgtzU7CUVsQzAEYIulzVkVFA95q0AEql8aAkk6EALw_wcB</t>
   </si>
   <si>
@@ -174,6 +171,21 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/6007</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/edatec/ED-PI5CASE-BS/21769634</t>
+  </si>
+  <si>
+    <t>Raspberry PI 4B case</t>
+  </si>
+  <si>
+    <t>Single Board Computer</t>
+  </si>
+  <si>
+    <t>case for Single Board Computer</t>
+  </si>
+  <si>
+    <t>Wireless transceivers</t>
   </si>
 </sst>
 </file>
@@ -593,30 +605,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D3A36C-E8CE-4E50-A172-E48E2F9A45A8}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.453125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="69.42578125" style="5" customWidth="1"/>
     <col min="8" max="8" width="76" style="5" customWidth="1"/>
-    <col min="9" max="9" width="83.54296875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="62.54296875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="55.81640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="83.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="62.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="55.85546875" style="5" customWidth="1"/>
     <col min="12" max="12" width="51" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="5"/>
+    <col min="13" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -648,7 +660,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,9 +684,9 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
@@ -689,25 +701,25 @@
         <v>50</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F10" si="0">C3*E3</f>
+        <f t="shared" ref="F3:F11" si="0">C3*E3</f>
         <v>50</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -716,28 +728,24 @@
         <v>23</v>
       </c>
       <c r="E4" s="3">
-        <v>3.95</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>3.95</v>
+        <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -746,22 +754,28 @@
         <v>23</v>
       </c>
       <c r="E5" s="3">
-        <v>8.23</v>
+        <v>3.95</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>8.23</v>
+        <v>3.95</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -770,29 +784,22 @@
         <v>23</v>
       </c>
       <c r="E6" s="3">
-        <v>6.6</v>
+        <v>8.23</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>6.6</v>
+        <v>8.23</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -801,25 +808,29 @@
         <v>23</v>
       </c>
       <c r="E7" s="3">
-        <v>0.2</v>
+        <v>6.6</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>6.6</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -828,25 +839,25 @@
         <v>23</v>
       </c>
       <c r="E8" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -855,76 +866,89 @@
         <v>23</v>
       </c>
       <c r="E9" s="3">
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="3">
-        <v>0.48</v>
+        <v>0.26</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="6">
-        <f>SUM(F2:F10)</f>
-        <v>96.960000000000008</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="6">
+        <f>SUM(F2:F11)</f>
+        <v>112.96000000000001</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -932,7 +956,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -946,7 +970,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -960,7 +984,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -974,7 +998,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -988,7 +1012,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1002,7 +1026,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1016,7 +1040,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1030,7 +1054,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1044,7 +1068,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1058,34 +1082,34 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1099,7 +1123,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1113,7 +1137,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" s="2" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1127,26 +1151,42 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
+    <row r="27" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" display="https://www.digikey.com/en/products/detail/american-opto-plus-led/L314ED/13677700?s=N4IgTCBcDaIDIGYCMAWAogERAXQL5A" xr:uid="{EB1FB783-CD78-4F2E-ADAE-2EFC2E0C050D}"/>
-    <hyperlink ref="G10" r:id="rId2" display="https://www.digikey.com/en/products/detail/kemet/c1206s104k5racauto/10232834" xr:uid="{CDDFAE49-11BE-4283-9E44-D17951ACE335}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{98CBDFFF-5BC0-4691-985C-193C55CD2A4F}"/>
-    <hyperlink ref="G9" r:id="rId4" xr:uid="{9AFC6348-0E57-4A67-A197-41D4FD45794D}"/>
-    <hyperlink ref="G6" r:id="rId5" display="https://www.digikey.com/en/products/detail/raspberry-pi/SC0339L/12339165?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLliTb25Erv6NiD1YUmheOuryx&amp;gclid=Cj0KCQjwvJHIBhCgARIsAEQnWlDQ6JN4eg4O2KvihoihYaPILt0_g-A7s0a8kHtxZmLVeqAIM-Sh0BoaAvo5EALw_wcB&amp;gclsrc=aw.ds" xr:uid="{61E141EF-661E-4EBA-8C6F-96D65CA0409E}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{60BE19F9-B00E-4A38-93C1-3776CD048CE8}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{3D5F3E6A-6737-45F8-8535-573468026212}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{95C484F2-35E3-4593-A56E-D63C69037E07}"/>
-    <hyperlink ref="H6" r:id="rId9" xr:uid="{347F1FD8-B28B-4914-AB8E-632B5A9DF65D}"/>
-    <hyperlink ref="I6" r:id="rId10" xr:uid="{44996A18-6D4F-4B97-A45D-678CF58A7F3D}"/>
+    <hyperlink ref="G8" r:id="rId1" display="https://www.digikey.com/en/products/detail/american-opto-plus-led/L314ED/13677700?s=N4IgTCBcDaIDIGYCMAWAogERAXQL5A" xr:uid="{EB1FB783-CD78-4F2E-ADAE-2EFC2E0C050D}"/>
+    <hyperlink ref="G11" r:id="rId2" display="https://www.digikey.com/en/products/detail/kemet/c1206s104k5racauto/10232834" xr:uid="{CDDFAE49-11BE-4283-9E44-D17951ACE335}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{98CBDFFF-5BC0-4691-985C-193C55CD2A4F}"/>
+    <hyperlink ref="G10" r:id="rId4" xr:uid="{9AFC6348-0E57-4A67-A197-41D4FD45794D}"/>
+    <hyperlink ref="G7" r:id="rId5" display="https://www.digikey.com/en/products/detail/raspberry-pi/SC0339L/12339165?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLliTb25Erv6NiD1YUmheOuryx&amp;gclid=Cj0KCQjwvJHIBhCgARIsAEQnWlDQ6JN4eg4O2KvihoihYaPILt0_g-A7s0a8kHtxZmLVeqAIM-Sh0BoaAvo5EALw_wcB&amp;gclsrc=aw.ds" xr:uid="{61E141EF-661E-4EBA-8C6F-96D65CA0409E}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{60BE19F9-B00E-4A38-93C1-3776CD048CE8}"/>
+    <hyperlink ref="H10" r:id="rId7" xr:uid="{3D5F3E6A-6737-45F8-8535-573468026212}"/>
+    <hyperlink ref="H11" r:id="rId8" xr:uid="{95C484F2-35E3-4593-A56E-D63C69037E07}"/>
+    <hyperlink ref="H7" r:id="rId9" xr:uid="{347F1FD8-B28B-4914-AB8E-632B5A9DF65D}"/>
+    <hyperlink ref="I7" r:id="rId10" xr:uid="{44996A18-6D4F-4B97-A45D-678CF58A7F3D}"/>
     <hyperlink ref="I3" r:id="rId11" xr:uid="{D562EEB9-C96C-430A-A068-DC1FB5CC4C0B}"/>
-    <hyperlink ref="G4" r:id="rId12" xr:uid="{08D8A779-6421-4A7D-93A0-92A87D2976CE}"/>
-    <hyperlink ref="H4" r:id="rId13" display="https://www.elecbee.com/en/product-detail/1100-meter-long-distance-nrf24l01-pa-lna-wireless-module-with-antenna-module_73275?utm_term=&amp;utm_campaign=&amp;utm_source=adwords&amp;utm_medium=ppc&amp;hsa_acc=9958698819&amp;hsa_cam=23146566611&amp;hsa_grp=187297116859&amp;hsa_ad=779498650524&amp;hsa_src=g&amp;hsa_tgt=pla-2511885727437&amp;hsa_kw=&amp;hsa_mt=&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gad_source=1&amp;gad_campaignid=23146566611&amp;gbraid=0AAAAADGHwHYfKF0iMEZtoqyx1rWjzHw1t&amp;gclid=Cj0KCQiA5abIBhCaARIsAM3-zFXbXR-v0fRxqHBuXN-ZMrGgtzU7CUVsQzAEYIulzVkVFA95q0AEql8aAkk6EALw_wcB" xr:uid="{51F6E1BD-05CB-4E6F-B0AD-45CBC164CA2B}"/>
-    <hyperlink ref="I4" r:id="rId14" xr:uid="{42ED7D58-C218-4B83-AF69-849F1693EE51}"/>
-    <hyperlink ref="G8" r:id="rId15" xr:uid="{567FA867-CBE5-4335-9DB4-2DB3C6277731}"/>
-    <hyperlink ref="H8" r:id="rId16" xr:uid="{A36A03ED-A124-4B3B-8FE2-AEA59150FA52}"/>
+    <hyperlink ref="G5" r:id="rId12" xr:uid="{08D8A779-6421-4A7D-93A0-92A87D2976CE}"/>
+    <hyperlink ref="H5" r:id="rId13" display="https://www.elecbee.com/en/product-detail/1100-meter-long-distance-nrf24l01-pa-lna-wireless-module-with-antenna-module_73275?utm_term=&amp;utm_campaign=&amp;utm_source=adwords&amp;utm_medium=ppc&amp;hsa_acc=9958698819&amp;hsa_cam=23146566611&amp;hsa_grp=187297116859&amp;hsa_ad=779498650524&amp;hsa_src=g&amp;hsa_tgt=pla-2511885727437&amp;hsa_kw=&amp;hsa_mt=&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gad_source=1&amp;gad_campaignid=23146566611&amp;gbraid=0AAAAADGHwHYfKF0iMEZtoqyx1rWjzHw1t&amp;gclid=Cj0KCQiA5abIBhCaARIsAM3-zFXbXR-v0fRxqHBuXN-ZMrGgtzU7CUVsQzAEYIulzVkVFA95q0AEql8aAkk6EALw_wcB" xr:uid="{51F6E1BD-05CB-4E6F-B0AD-45CBC164CA2B}"/>
+    <hyperlink ref="I5" r:id="rId14" xr:uid="{42ED7D58-C218-4B83-AF69-849F1693EE51}"/>
+    <hyperlink ref="G9" r:id="rId15" xr:uid="{567FA867-CBE5-4335-9DB4-2DB3C6277731}"/>
+    <hyperlink ref="H9" r:id="rId16" xr:uid="{A36A03ED-A124-4B3B-8FE2-AEA59150FA52}"/>
+    <hyperlink ref="G3" r:id="rId17" xr:uid="{5F161355-9104-4121-A6E5-DCB52D413780}"/>
+    <hyperlink ref="G4" r:id="rId18" xr:uid="{74708F2C-38FA-40F7-B94E-BFB0E11AFC7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EDA files added, BOM modified, Readme updated
</commit_message>
<xml_diff>
--- a/system_development/V0.3.1/bill_of_materials.xlsx
+++ b/system_development/V0.3.1/bill_of_materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailsc-my.sharepoint.com/personal/asifuzzaman_sc_edu/Documents/Github Repos/Sensor-Package-Access-Hub/system_development/V0.3.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="13_ncr:1_{92FC9251-22EE-4CB6-81B0-D0434CABC585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9D1CE0F-ADD6-4866-A8C4-8DC3E3E444C0}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{92FC9251-22EE-4CB6-81B0-D0434CABC585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD7D508F-5A6A-4073-9614-A059371260B6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
+    <workbookView xWindow="28680" yWindow="-22170" windowWidth="16440" windowHeight="28320" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="bill_of_materials" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,9 @@
     <t>Arduino Nano</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>Resistors</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Designator</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
@@ -71,18 +62,9 @@
     <t>https://oshpark.com/</t>
   </si>
   <si>
-    <t>Capacitors 0.1uF</t>
-  </si>
-  <si>
-    <t>Capacitor 10uF</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECE-A1EKS100B/2689095</t>
   </si>
   <si>
-    <t>ECE-A1EKS100B</t>
-  </si>
-  <si>
     <t>Vendor 1</t>
   </si>
   <si>
@@ -125,21 +107,12 @@
     <t>https://www.cdw.com/product/sandisk-extreme-flash-memory-card-64-gb-microsdxc-uhs-i/7316165?pfm=srh</t>
   </si>
   <si>
-    <t>L314ED 3mm RED</t>
-  </si>
-  <si>
-    <t>DC-DC converter</t>
-  </si>
-  <si>
     <t>5V to 3.3V buck converter</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Raspberry-Pi/SC01949?qs=T%252BzbugeAwjjISb%252BwlagpRw%3D%3D</t>
   </si>
   <si>
-    <t>NRF24</t>
-  </si>
-  <si>
     <t>https://www.elecbee.com/en/product-detail/1100-meter-long-distance-nrf24l01-pa-lna-wireless-module-with-antenna-module_73275?utm_term=&amp;utm_campaign=&amp;utm_source=adwords&amp;utm_medium=ppc&amp;hsa_acc=9958698819&amp;hsa_cam=23146566611&amp;hsa_grp=187297116859&amp;hsa_ad=779498650524&amp;hsa_src=g&amp;hsa_tgt=pla-2511885727437&amp;hsa_kw=&amp;hsa_mt=&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gad_source=1&amp;gad_campaignid=23146566611&amp;gbraid=0AAAAADGHwHYfKF0iMEZtoqyx1rWjzHw1t&amp;gclid=Cj0KCQiA5abIBhCaARIsAM3-zFXbXR-v0fRxqHBuXN-ZMrGgtzU7CUVsQzAEYIulzVkVFA95q0AEql8aAkk6EALw_wcB</t>
   </si>
   <si>
@@ -149,27 +122,12 @@
     <t>https://openelab.io/products/nrf24l01-transceiver-transceiver-module?srsltid=AfmBOorW9lfupEOXFS3kU72MZQgoLedxFpkylsIVPOrEJnmP53qSnV0F</t>
   </si>
   <si>
-    <t>RES 270 OHM 5% 1/4W AXIAL</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CF14JT270R/1741362</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/YAGEO/CFR25SJT-26-270R?qs=sGAEpiMZZMsPqMdJzcrNwjRWpSA1Ui8vfWaBDCu2IB3jHFqFn4CeHg%3D%3D</t>
-  </si>
-  <si>
-    <t>C1206S104K5RACAUTO,  0.1 µF ±10% 50V Ceramic Capacitor X7R 1206 (3216 Metric)</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/raspberry-pi/SC1642/24627138</t>
   </si>
   <si>
     <t>https://www.adafruit.com/product/6007</t>
   </si>
   <si>
-    <t>5.1V 5A adapter for PI</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/raspberry-pi/SC1153/21658276?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLlhBKp1jjVV0wK9-_mClnX9Xb&amp;gclid=CjwKCAiAt8bIBhBpEiwAzH1w6XiWYkHlYnY4a9hNgAJ6HaS7k8nBn525TTe7Kp73m9FFLnfHdqppzxoCku4QAvD_BwE</t>
   </si>
   <si>
@@ -179,9 +137,6 @@
     <t>Raspberry PI 5, 2GB RAM</t>
   </si>
   <si>
-    <t>64 / 32 GB MicroSD card</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/COM-18357/15189221?gclsrc=aw.ds&amp;gad_source=4&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlj6-1mOsbENDPcdOfYHIOlTf&amp;gclid=CjwKCAiA2svIBhB-EiwARWDPjphR8Mo50YVUvb1N4wZHW3ESAzcPcqV9oUoAIf9KWH-_yjsUEWJWoxoC4GkQAvD_BwE</t>
   </si>
   <si>
@@ -189,6 +144,51 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/universal-solder-electronics-ltd/26014/26606379?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLliYomKhH2MAZtF1d7mkzJeC-&amp;gclid=CjwKCAiA2svIBhB-EiwARWDPjjHxiD5wOUWqZL3fssPYD2OiHsmO0L69KLIBtITF0j5OwLV159JyrRoCS34QAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF1206JT270R/1757430</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF1206FT270R/1759786</t>
+  </si>
+  <si>
+    <t>270 Ohms ±5% 0.25W, 1/4W Chip Resistor 1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>PCB Designator</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C1, 2, 3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>DC-DC buck</t>
+  </si>
+  <si>
+    <t>nRF24</t>
+  </si>
+  <si>
+    <t>3mm Red 620nm LED Indication - Discrete 1.85V Radial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64 / 32 GB MicroSD card </t>
+  </si>
+  <si>
+    <t>0.1 µF ±10% 50V Ceramic Capacitor X7R 1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>5.1V 5A PD USB-C adapter for PI</t>
+  </si>
+  <si>
+    <t>10 µF 25 V Aluminum Electrolytic Capacitor Radial</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,31 +633,31 @@
   <sheetData>
     <row r="1" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3">
         <v>10.89</v>
@@ -684,23 +684,23 @@
         <v>10.89</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3">
         <v>12</v>
@@ -710,25 +710,25 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3">
         <v>50</v>
@@ -738,27 +738,27 @@
         <v>50</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3">
         <v>4.95</v>
@@ -768,25 +768,25 @@
         <v>4.95</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3">
         <v>3.95</v>
@@ -796,27 +796,27 @@
         <v>3.95</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3">
         <v>8.23</v>
@@ -826,12 +826,12 @@
         <v>8.23</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>47</v>
@@ -840,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3">
         <v>6.6</v>
@@ -850,28 +850,28 @@
         <v>6.6</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3">
         <v>0.2</v>
@@ -881,24 +881,24 @@
         <v>0.2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3">
         <v>0.1</v>
@@ -908,24 +908,24 @@
         <v>0.1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3">
         <v>0.26</v>
@@ -935,24 +935,24 @@
         <v>0.26</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3">
         <v>0.48</v>
@@ -962,10 +962,10 @@
         <v>0.96</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -974,7 +974,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" s="6">
         <f>SUM(F2:F12)</f>
@@ -1212,15 +1212,15 @@
     <hyperlink ref="G6" r:id="rId12" xr:uid="{08D8A779-6421-4A7D-93A0-92A87D2976CE}"/>
     <hyperlink ref="H6" r:id="rId13" display="https://www.elecbee.com/en/product-detail/1100-meter-long-distance-nrf24l01-pa-lna-wireless-module-with-antenna-module_73275?utm_term=&amp;utm_campaign=&amp;utm_source=adwords&amp;utm_medium=ppc&amp;hsa_acc=9958698819&amp;hsa_cam=23146566611&amp;hsa_grp=187297116859&amp;hsa_ad=779498650524&amp;hsa_src=g&amp;hsa_tgt=pla-2511885727437&amp;hsa_kw=&amp;hsa_mt=&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gad_source=1&amp;gad_campaignid=23146566611&amp;gbraid=0AAAAADGHwHYfKF0iMEZtoqyx1rWjzHw1t&amp;gclid=Cj0KCQiA5abIBhCaARIsAM3-zFXbXR-v0fRxqHBuXN-ZMrGgtzU7CUVsQzAEYIulzVkVFA95q0AEql8aAkk6EALw_wcB" xr:uid="{51F6E1BD-05CB-4E6F-B0AD-45CBC164CA2B}"/>
     <hyperlink ref="I6" r:id="rId14" xr:uid="{42ED7D58-C218-4B83-AF69-849F1693EE51}"/>
-    <hyperlink ref="G10" r:id="rId15" xr:uid="{567FA867-CBE5-4335-9DB4-2DB3C6277731}"/>
-    <hyperlink ref="H10" r:id="rId16" xr:uid="{A36A03ED-A124-4B3B-8FE2-AEA59150FA52}"/>
-    <hyperlink ref="G3" r:id="rId17" display="https://www.digikey.com/en/products/detail/raspberry-pi/SC1153/21658276?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLlhBKp1jjVV0wK9-_mClnX9Xb&amp;gclid=CjwKCAiAt8bIBhBpEiwAzH1w6XiWYkHlYnY4a9hNgAJ6HaS7k8nBn525TTe7Kp73m9FFLnfHdqppzxoCku4QAvD_BwE" xr:uid="{8B23B937-1C13-4161-9664-DD5F24C70088}"/>
-    <hyperlink ref="G4" r:id="rId18" xr:uid="{D64E76CC-9EC1-41FF-948D-E7CF6CBCA441}"/>
-    <hyperlink ref="H3" r:id="rId19" xr:uid="{B2E43AAD-E6ED-43A2-BCAA-9D754B46D9FF}"/>
-    <hyperlink ref="H4" r:id="rId20" xr:uid="{CA43E14C-2D0F-4301-8844-C3295C6EDA87}"/>
-    <hyperlink ref="G5" r:id="rId21" display="https://www.digikey.com/en/products/detail/sparkfun-electronics/COM-18357/15189221?gclsrc=aw.ds&amp;gad_source=4&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlj6-1mOsbENDPcdOfYHIOlTf&amp;gclid=CjwKCAiA2svIBhB-EiwARWDPjphR8Mo50YVUvb1N4wZHW3ESAzcPcqV9oUoAIf9KWH-_yjsUEWJWoxoC4GkQAvD_BwE" xr:uid="{8C766155-CE0C-4BD6-A255-DEB4F053A106}"/>
-    <hyperlink ref="H5" r:id="rId22" xr:uid="{9CFD84EE-A7A6-49A0-BDF5-18D690BECBA5}"/>
-    <hyperlink ref="G2" r:id="rId23" display="https://www.digikey.com/en/products/detail/universal-solder-electronics-ltd/26014/26606379?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLliYomKhH2MAZtF1d7mkzJeC-&amp;gclid=CjwKCAiA2svIBhB-EiwARWDPjjHxiD5wOUWqZL3fssPYD2OiHsmO0L69KLIBtITF0j5OwLV159JyrRoCS34QAvD_BwE" xr:uid="{52DDE32A-61FC-41BB-8F21-9A22BB687B9B}"/>
+    <hyperlink ref="G3" r:id="rId15" display="https://www.digikey.com/en/products/detail/raspberry-pi/SC1153/21658276?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLlhBKp1jjVV0wK9-_mClnX9Xb&amp;gclid=CjwKCAiAt8bIBhBpEiwAzH1w6XiWYkHlYnY4a9hNgAJ6HaS7k8nBn525TTe7Kp73m9FFLnfHdqppzxoCku4QAvD_BwE" xr:uid="{8B23B937-1C13-4161-9664-DD5F24C70088}"/>
+    <hyperlink ref="G4" r:id="rId16" xr:uid="{D64E76CC-9EC1-41FF-948D-E7CF6CBCA441}"/>
+    <hyperlink ref="H3" r:id="rId17" xr:uid="{B2E43AAD-E6ED-43A2-BCAA-9D754B46D9FF}"/>
+    <hyperlink ref="H4" r:id="rId18" xr:uid="{CA43E14C-2D0F-4301-8844-C3295C6EDA87}"/>
+    <hyperlink ref="G5" r:id="rId19" display="https://www.digikey.com/en/products/detail/sparkfun-electronics/COM-18357/15189221?gclsrc=aw.ds&amp;gad_source=4&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlj6-1mOsbENDPcdOfYHIOlTf&amp;gclid=CjwKCAiA2svIBhB-EiwARWDPjphR8Mo50YVUvb1N4wZHW3ESAzcPcqV9oUoAIf9KWH-_yjsUEWJWoxoC4GkQAvD_BwE" xr:uid="{8C766155-CE0C-4BD6-A255-DEB4F053A106}"/>
+    <hyperlink ref="H5" r:id="rId20" xr:uid="{9CFD84EE-A7A6-49A0-BDF5-18D690BECBA5}"/>
+    <hyperlink ref="G2" r:id="rId21" display="https://www.digikey.com/en/products/detail/universal-solder-electronics-ltd/26014/26606379?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLliYomKhH2MAZtF1d7mkzJeC-&amp;gclid=CjwKCAiA2svIBhB-EiwARWDPjjHxiD5wOUWqZL3fssPYD2OiHsmO0L69KLIBtITF0j5OwLV159JyrRoCS34QAvD_BwE" xr:uid="{52DDE32A-61FC-41BB-8F21-9A22BB687B9B}"/>
+    <hyperlink ref="G10" r:id="rId22" xr:uid="{8A560E40-7FBD-4E0E-8D4A-A72DAFFAFCC4}"/>
+    <hyperlink ref="H10" r:id="rId23" xr:uid="{38A3F040-F64B-4A41-9FA1-10FB31827F59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>

</xml_diff>